<commit_message>
update the truth table with the Priority Lamp
</commit_message>
<xml_diff>
--- a/Verilog/Thesis_FPGA_Traffic_Light/Trust_Table/Trust_Table.xlsx
+++ b/Verilog/Thesis_FPGA_Traffic_Light/Trust_Table/Trust_Table.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Place\Thesis_FPGA\Trust_Table\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Place\Practice_space\Practice_SP\Verilog\Thesis_FPGA_Traffic_Light\Trust_Table\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="State machine" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>State machine</t>
   </si>
@@ -145,13 +145,19 @@
     <t>Street B</t>
   </si>
   <si>
-    <t>State Đèn</t>
-  </si>
-  <si>
     <t>ON</t>
   </si>
   <si>
     <t>OFF</t>
+  </si>
+  <si>
+    <t>State đèn ưu tiên</t>
+  </si>
+  <si>
+    <t>Trạng thái đèn ưu tiên</t>
+  </si>
+  <si>
+    <t>Priority lamp</t>
   </si>
 </sst>
 </file>
@@ -187,7 +193,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -223,26 +229,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -260,15 +363,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>447674</xdr:colOff>
+      <xdr:colOff>447673</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>513985</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -277,8 +380,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="447674" y="1247775"/>
-          <a:ext cx="990600" cy="361950"/>
+          <a:off x="447673" y="1247775"/>
+          <a:ext cx="1028337" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -310,6 +413,47 @@
             <a:t>AG_BR</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>APL_OFF</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BPL_ON</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -317,15 +461,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:colOff>523874</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>723536</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -334,8 +478,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2800350" y="1247775"/>
-          <a:ext cx="990600" cy="361950"/>
+          <a:off x="2800349" y="1247775"/>
+          <a:ext cx="1028337" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -367,6 +511,42 @@
             <a:t>AY_BR</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>APL_OFF</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BPL_ON</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -380,9 +560,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1000124</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1038224</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -392,7 +572,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5343524" y="1247775"/>
-          <a:ext cx="1000125" cy="361950"/>
+          <a:ext cx="1038225" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -424,6 +604,42 @@
             <a:t>AR_BR1</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>APL_ON</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BPL_OFF</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -432,14 +648,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1038225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -448,8 +664,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5343525" y="2314575"/>
-          <a:ext cx="1000125" cy="361950"/>
+          <a:off x="5343525" y="3095625"/>
+          <a:ext cx="1038225" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -481,6 +697,39 @@
             <a:t>AR_BG</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>APL_OFF</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BPL_ON</a:t>
+          </a:r>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -489,14 +738,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -505,8 +754,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2790825" y="2314575"/>
-          <a:ext cx="1000125" cy="361950"/>
+          <a:off x="2790825" y="3095625"/>
+          <a:ext cx="1038225" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -538,6 +787,42 @@
             <a:t>AR_BY</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>APL_OFF</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BPL_ON</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -545,15 +830,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>503735</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -562,8 +847,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="457200" y="2314575"/>
-          <a:ext cx="971550" cy="361950"/>
+          <a:off x="457199" y="3095625"/>
+          <a:ext cx="1008561" cy="1047750"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -595,6 +880,42 @@
             <a:t>AR_BR2</a:t>
           </a:r>
         </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>APL_ON</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>BPL_OFF</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
       </xdr:txBody>
     </xdr:sp>
     <xdr:clientData/>
@@ -602,15 +923,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>513985</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -622,8 +943,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1438274" y="1428750"/>
-          <a:ext cx="1362076" cy="0"/>
+          <a:off x="1476010" y="1771650"/>
+          <a:ext cx="1324339" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -652,15 +973,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>723536</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>761999</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -672,8 +993,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3790950" y="1428750"/>
-          <a:ext cx="1552574" cy="0"/>
+          <a:off x="3828686" y="1771650"/>
+          <a:ext cx="1514838" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -702,15 +1023,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>519112</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>500063</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>519113</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -722,8 +1043,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5843587" y="1609725"/>
-          <a:ext cx="1" cy="704850"/>
+          <a:off x="5862637" y="2295525"/>
+          <a:ext cx="1" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -752,15 +1073,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -772,8 +1093,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3790950" y="2495550"/>
-          <a:ext cx="1552575" cy="0"/>
+          <a:off x="3829050" y="3619500"/>
+          <a:ext cx="1514475" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -802,15 +1123,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>503735</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -822,8 +1143,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1428750" y="2495550"/>
-          <a:ext cx="1362075" cy="0"/>
+          <a:off x="1465760" y="3619500"/>
+          <a:ext cx="1325065" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -852,15 +1173,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>928687</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>961480</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>928688</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>961842</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -871,9 +1192,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="928687" y="1609725"/>
-          <a:ext cx="1" cy="704850"/>
+        <a:xfrm flipV="1">
+          <a:off x="961480" y="2295525"/>
+          <a:ext cx="362" cy="800100"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -902,15 +1223,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -919,7 +1240,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1476375" y="1123950"/>
+          <a:off x="1504950" y="1362075"/>
           <a:ext cx="1133475" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -964,16 +1285,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -982,7 +1303,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3905250" y="1123950"/>
+          <a:off x="3886200" y="1343025"/>
           <a:ext cx="1323975" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1024,15 +1345,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1041,7 +1362,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5876925" y="1790700"/>
+          <a:off x="5734050" y="2514600"/>
           <a:ext cx="885825" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1083,15 +1404,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1100,7 +1421,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3943350" y="2219325"/>
+          <a:off x="3933825" y="3343275"/>
           <a:ext cx="1323975" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1141,16 +1462,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1159,7 +1480,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1695450" y="2228850"/>
+          <a:off x="1609725" y="3305175"/>
           <a:ext cx="990600" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1201,15 +1522,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1218,7 +1539,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="866775" y="1800225"/>
+          <a:off x="781050" y="2562225"/>
           <a:ext cx="1028700" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1260,15 +1581,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>928687</xdr:colOff>
+      <xdr:colOff>961843</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>326994</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>100631</xdr:rowOff>
+      <xdr:colOff>363390</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1039</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1280,12 +1601,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="1082350" y="1094112"/>
-          <a:ext cx="53006" cy="360332"/>
+          <a:off x="1066909" y="1142709"/>
+          <a:ext cx="153439" cy="363572"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 531272"/>
+            <a:gd name="adj1" fmla="val 248984"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1312,15 +1633,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
+      <xdr:colOff>209369</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>540730</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>100631</xdr:rowOff>
+      <xdr:colOff>572941</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1039</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1332,12 +1653,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="3444262" y="1099163"/>
-          <a:ext cx="53006" cy="350230"/>
+          <a:off x="3419585" y="1142709"/>
+          <a:ext cx="153439" cy="363572"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 531272"/>
+            <a:gd name="adj1" fmla="val 248984"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1364,15 +1685,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>500062</xdr:colOff>
+      <xdr:colOff>519113</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>853659</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>100631</xdr:rowOff>
+      <xdr:colOff>886180</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1039</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1384,12 +1705,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="5993883" y="1097479"/>
-          <a:ext cx="53006" cy="353597"/>
+          <a:off x="5969452" y="1140961"/>
+          <a:ext cx="153439" cy="367067"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 531272"/>
+            <a:gd name="adj1" fmla="val 248984"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1416,15 +1737,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>853659</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>886179</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1000124</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>23194</xdr:rowOff>
+      <xdr:colOff>1038224</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>189461</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1436,13 +1757,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1" flipV="1">
-          <a:off x="6206432" y="2486302"/>
-          <a:ext cx="127969" cy="146465"/>
+          <a:off x="6120509" y="3728695"/>
+          <a:ext cx="370436" cy="152045"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -220058"/>
-            <a:gd name="adj2" fmla="val 256078"/>
+            <a:gd name="adj1" fmla="val -103132"/>
+            <a:gd name="adj2" fmla="val 250350"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1469,15 +1790,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>185738</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>204789</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>539335</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>167306</xdr:rowOff>
+      <xdr:colOff>571856</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>48664</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1489,12 +1810,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipV="1">
-          <a:off x="3441184" y="2164279"/>
-          <a:ext cx="53006" cy="353597"/>
+          <a:off x="3416753" y="2988811"/>
+          <a:ext cx="153439" cy="367067"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 531272"/>
+            <a:gd name="adj1" fmla="val 248984"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1521,15 +1842,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95251</xdr:rowOff>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>603665</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>23195</xdr:rowOff>
+      <xdr:colOff>604899</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>189461</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1541,13 +1862,13 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000" flipH="1">
-          <a:off x="466448" y="2486303"/>
-          <a:ext cx="127969" cy="146465"/>
+          <a:off x="345831" y="3730868"/>
+          <a:ext cx="370436" cy="147700"/>
         </a:xfrm>
         <a:prstGeom prst="curvedConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -220058"/>
-            <a:gd name="adj2" fmla="val 256078"/>
+            <a:gd name="adj1" fmla="val -103132"/>
+            <a:gd name="adj2" fmla="val 254773"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1634,9 +1955,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>592744</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>100631</xdr:rowOff>
+      <xdr:colOff>598269</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1039</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1649,7 +1970,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="405828" y="933888"/>
-          <a:ext cx="186916" cy="366893"/>
+          <a:ext cx="192441" cy="467326"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1730,6 +2051,126 @@
             <a:t>Init state</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="TextBox 54"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7029450" y="1219200"/>
+          <a:ext cx="2886075" cy="1314450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng"/>
+            <a:t>Chú</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" u="sng" baseline="0"/>
+            <a:t> thích:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>A*: đường A, * = R,G,Y - RED, GREEN, YELLOW</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>B*: đường B, * = R,G,Y - RED, GREEN, YELLOW</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>APL_*: Đèn ưu tiên đường A</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>BPL_*: Đèn ưu tiên đường B</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2003,7 +2444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2032,7 +2475,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2047,6 +2492,7 @@
     <col min="12" max="12" width="6.125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.25" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2059,13 +2505,8 @@
       <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q4" s="1" t="s">
-        <v>40</v>
+      <c r="Q3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2123,7 +2564,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="1" t="str">
-        <f>CONCATENATE("0b",DEC2BIN(D6,3))</f>
+        <f t="shared" ref="E6:E11" si="0">CONCATENATE("0b",DEC2BIN(D6,3))</f>
         <v>0b000</v>
       </c>
       <c r="F6" s="1" t="str">
@@ -2152,6 +2593,9 @@
       </c>
       <c r="O6" s="1">
         <v>29</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -2168,19 +2612,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="1" t="str">
-        <f>CONCATENATE("0b",DEC2BIN(D7,3))</f>
+        <f t="shared" si="0"/>
         <v>0b001</v>
       </c>
       <c r="F7" s="1" t="str">
-        <f t="shared" ref="F7:F11" si="0">MID($E7,3,1)</f>
+        <f t="shared" ref="F7:F11" si="1">MID($E7,3,1)</f>
         <v>0</v>
       </c>
       <c r="G7" s="1" t="str">
-        <f t="shared" ref="G7:G11" si="1">MID($E7,4,1)</f>
+        <f t="shared" ref="G7:G11" si="2">MID($E7,4,1)</f>
         <v>0</v>
       </c>
       <c r="H7" s="1" t="str">
-        <f t="shared" ref="H7:H11" si="2">MID($E7,5,1)</f>
+        <f t="shared" ref="H7:H11" si="3">MID($E7,5,1)</f>
         <v>1</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -2197,6 +2641,9 @@
       </c>
       <c r="O7" s="1">
         <v>4</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -2213,19 +2660,19 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="str">
-        <f>CONCATENATE("0b",DEC2BIN(D8,3))</f>
+        <f t="shared" si="0"/>
         <v>0b010</v>
       </c>
       <c r="F8" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G8" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H8" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -2249,19 +2696,19 @@
         <v>3</v>
       </c>
       <c r="E9" s="1" t="str">
-        <f>CONCATENATE("0b",DEC2BIN(D9,3))</f>
+        <f t="shared" si="0"/>
         <v>0b011</v>
       </c>
       <c r="F9" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G9" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H9" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -2285,19 +2732,19 @@
         <v>4</v>
       </c>
       <c r="E10" s="1" t="str">
-        <f>CONCATENATE("0b",DEC2BIN(D10,3))</f>
+        <f t="shared" si="0"/>
         <v>0b100</v>
       </c>
       <c r="F10" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G10" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J10" s="4" t="s">
@@ -2324,19 +2771,19 @@
         <v>5</v>
       </c>
       <c r="E11" s="1" t="str">
-        <f>CONCATENATE("0b",DEC2BIN(D11,3))</f>
+        <f t="shared" si="0"/>
         <v>0b101</v>
       </c>
       <c r="F11" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G11" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H11" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J11" s="4" t="s">
@@ -2386,40 +2833,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:N11"/>
+  <dimension ref="A4:P11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6" t="s">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
@@ -2444,26 +2897,32 @@
       <c r="H5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="N5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="O5" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="P5" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -2507,19 +2966,27 @@
         <v>OFF</v>
       </c>
       <c r="L6" s="1" t="str">
+        <f>IF(OR(I6="ON",J6="ON"),"OFF","ON")</f>
+        <v>OFF</v>
+      </c>
+      <c r="M6" s="1" t="str">
         <f>IF($A6="AR_BG","ON","OFF")</f>
         <v>OFF</v>
       </c>
-      <c r="M6" s="1" t="str">
+      <c r="N6" s="1" t="str">
         <f>IF($A6="AR_BY","ON","OFF")</f>
         <v>OFF</v>
       </c>
-      <c r="N6" s="1" t="str">
+      <c r="O6" s="1" t="str">
         <f>IF(AND($A6 &lt;&gt; "AR_BG", $A6 &lt;&gt; "AR_BY"), "ON", "OFF")</f>
         <v>ON</v>
       </c>
+      <c r="P6" s="1" t="str">
+        <f>IF(OR(M6="ON",N6="ON"),"OFF","ON")</f>
+        <v>ON</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -2555,7 +3022,7 @@
         <v>OFF</v>
       </c>
       <c r="J7" s="1" t="str">
-        <f t="shared" ref="J7:J11" si="1">IF($A7="AY_BR","ON","OFF")</f>
+        <f t="shared" ref="J7:J10" si="1">IF($A7="AY_BR","ON","OFF")</f>
         <v>ON</v>
       </c>
       <c r="K7" s="1" t="str">
@@ -2563,19 +3030,27 @@
         <v>OFF</v>
       </c>
       <c r="L7" s="1" t="str">
-        <f t="shared" ref="L7:L11" si="3">IF($A7="AR_BG","ON","OFF")</f>
+        <f t="shared" ref="L7:L11" si="3">IF(OR(I7="ON",J7="ON"),"OFF","ON")</f>
         <v>OFF</v>
       </c>
       <c r="M7" s="1" t="str">
-        <f t="shared" ref="M7:M11" si="4">IF($A7="AR_BY","ON","OFF")</f>
+        <f t="shared" ref="M7:M11" si="4">IF($A7="AR_BG","ON","OFF")</f>
         <v>OFF</v>
       </c>
       <c r="N7" s="1" t="str">
-        <f t="shared" ref="N7:N11" si="5">IF(AND($A7 &lt;&gt; "AR_BG", $A7 &lt;&gt; "AR_BY"), "ON", "OFF")</f>
+        <f t="shared" ref="N7:N11" si="5">IF($A7="AR_BY","ON","OFF")</f>
+        <v>OFF</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" ref="O7:O11" si="6">IF(AND($A7 &lt;&gt; "AR_BG", $A7 &lt;&gt; "AR_BY"), "ON", "OFF")</f>
         <v>ON</v>
       </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" ref="P7:P11" si="7">IF(OR(M7="ON",N7="ON"),"OFF","ON")</f>
+        <v>ON</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -2620,7 +3095,7 @@
       </c>
       <c r="L8" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>OFF</v>
+        <v>ON</v>
       </c>
       <c r="M8" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2628,10 +3103,18 @@
       </c>
       <c r="N8" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>OFF</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>ON</v>
       </c>
+      <c r="P8" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>ON</v>
+      </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -2680,14 +3163,22 @@
       </c>
       <c r="M9" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>OFF</v>
+        <v>ON</v>
       </c>
       <c r="N9" s="1" t="str">
         <f t="shared" si="5"/>
         <v>OFF</v>
       </c>
+      <c r="O9" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>OFF</v>
+      </c>
+      <c r="P9" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>OFF</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -2732,18 +3223,26 @@
       </c>
       <c r="L10" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>OFF</v>
+        <v>ON</v>
       </c>
       <c r="M10" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>ON</v>
+        <v>OFF</v>
       </c>
       <c r="N10" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>ON</v>
+      </c>
+      <c r="O10" s="1" t="str">
+        <f t="shared" si="6"/>
         <v>OFF</v>
       </c>
+      <c r="P10" s="1" t="str">
+        <f t="shared" si="7"/>
+        <v>OFF</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -2788,7 +3287,7 @@
       </c>
       <c r="L11" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>OFF</v>
+        <v>ON</v>
       </c>
       <c r="M11" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2796,6 +3295,14 @@
       </c>
       <c r="N11" s="1" t="str">
         <f t="shared" si="5"/>
+        <v>OFF</v>
+      </c>
+      <c r="O11" s="1" t="str">
+        <f t="shared" si="6"/>
+        <v>ON</v>
+      </c>
+      <c r="P11" s="1" t="str">
+        <f t="shared" si="7"/>
         <v>ON</v>
       </c>
     </row>
@@ -2803,10 +3310,51 @@
   <mergeCells count="4">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="M4:P4"/>
   </mergeCells>
+  <conditionalFormatting sqref="I6:I11">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J6:J11">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6:K11">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L6:L11">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6:M11">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N6:N11">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:O11">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P6:P11">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"ON"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>

<commit_message>
update the Traffic light thesis
</commit_message>
<xml_diff>
--- a/Verilog/Thesis_FPGA_Traffic_Light/Trust_Table/Trust_Table.xlsx
+++ b/Verilog/Thesis_FPGA_Traffic_Light/Trust_Table/Trust_Table.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12420"/>
+    <workbookView xWindow="1890" yWindow="0" windowWidth="28800" windowHeight="12420"/>
   </bookViews>
   <sheets>
     <sheet name="State machine" sheetId="1" r:id="rId1"/>
     <sheet name="Bảng quy định" sheetId="2" r:id="rId2"/>
     <sheet name="Trust table" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -163,7 +163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -281,7 +281,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -328,13 +328,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1894,16 +1887,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1912,7 +1905,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="161925" y="714375"/>
+          <a:off x="4981575" y="485775"/>
           <a:ext cx="285750" cy="257175"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
@@ -1948,14 +1941,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>405828</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>133788</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>598269</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>152044</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>1039</xdr:rowOff>
     </xdr:to>
@@ -1963,14 +1956,14 @@
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="65" name="Straight Arrow Connector 64"/>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="63" idx="5"/>
-          <a:endCxn id="2" idx="1"/>
+          <a:stCxn id="63" idx="4"/>
+          <a:endCxn id="4" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="405828" y="933888"/>
-          <a:ext cx="192441" cy="467326"/>
+          <a:off x="5124450" y="742950"/>
+          <a:ext cx="371119" cy="658264"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1998,16 +1991,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2016,7 +2009,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304800" y="628650"/>
+          <a:off x="4972050" y="457200"/>
           <a:ext cx="1133475" cy="285750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2445,7 +2438,7 @@
   <dimension ref="A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>